<commit_message>
Excel spreadsheet with 300 examples of riuscire v. potere.
</commit_message>
<xml_diff>
--- a/Riuscire_Potere/Riescare-Potere.xlsx
+++ b/Riuscire_Potere/Riescare-Potere.xlsx
@@ -936,7 +936,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -946,6 +946,12 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
@@ -970,17 +976,31 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1029,14 +1049,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:B301" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:B301" totalsRowShown="0" headerRowDxfId="0">
   <autoFilter ref="A1:B301"/>
   <sortState ref="A2:B301">
     <sortCondition ref="B1:B301"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" name="Italiano" dataDxfId="1"/>
-    <tableColumn id="3" name="Order" dataDxfId="0"/>
+    <tableColumn id="1" name="Italiano" dataDxfId="2"/>
+    <tableColumn id="3" name="Order" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1307,8 +1327,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B301"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A196" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1317,11 +1337,11 @@
     <col min="2" max="2" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>